<commit_message>
testing barcode reader 3
</commit_message>
<xml_diff>
--- a/JKMapp/static/counter_info.xlsx
+++ b/JKMapp/static/counter_info.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -423,7 +423,7 @@
   <sheetData>
     <row r="1">
       <c r="E1" t="n">
-        <v>12</v>
+        <v>17</v>
       </c>
     </row>
     <row r="2">
@@ -495,6 +495,42 @@
       <c r="D5" t="inlineStr">
         <is>
           <t>20:12:04</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" t="n">
+        <v>4</v>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>16-03-2024</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>00:31:13</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" t="n">
+        <v>1</v>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>16-03-2024</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>01:57:58</t>
         </is>
       </c>
     </row>

</xml_diff>